<commit_message>
update scattering and pmrms features
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussema\Desktop\codes\pattern\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tumde-my.sharepoint.com/personal/oussema_dhaouadi_tum_de/Documents/TUM/9th Semester (NTU)/PR&amp;ML/Project/CapsGeR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171B8EA6-A37E-456C-A421-ACEAFF9CA924}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="453" documentId="13_ncr:1_{D8CBC880-66BC-4602-A558-8BF04119AC51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8AF3A55D-5F70-4EE8-996E-A7A4C3D2EB43}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="27977" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7826" yWindow="5023" windowWidth="15969" windowHeight="9814" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="232">
   <si>
     <t>fcnet</t>
   </si>
@@ -150,12 +150,6 @@
   </si>
   <si>
     <t>65.67 (8)</t>
-  </si>
-  <si>
-    <t>not yet</t>
-  </si>
-  <si>
-    <t>fail</t>
   </si>
   <si>
     <t>Variable Window Dataset</t>
@@ -168,9 +162,6 @@
 Surface Electromyography Signals</t>
   </si>
   <si>
-    <t>https://www.mdpi.com/1424-8220/20/3/672</t>
-  </si>
-  <si>
     <t>Surface EMG Decoding for Hand Gestures Based on Spectrogram and
 CNN-LSTM*</t>
   </si>
@@ -179,9 +170,6 @@
   </si>
   <si>
     <t>DB2</t>
-  </si>
-  <si>
-    <t>https://ieeexplore.ieee.org/stamp/stamp.jsp?tp=&amp;arnumber=8630679</t>
   </si>
   <si>
     <t>Deep Learning for Electromyographic Hand
@@ -189,12 +177,6 @@
 Transfer Learning</t>
   </si>
   <si>
-    <t xml:space="preserve">DB5 41mov </t>
-  </si>
-  <si>
-    <t>https://ieeexplore.ieee.org/stamp/stamp.jsp?tp=&amp;arnumber=8983049</t>
-  </si>
-  <si>
     <t>Deep Neural Network Approach for Hand, Wrist,
 Grasping and Functional Movements Classification
 using Low-cost sEMG Sensors</t>
@@ -203,16 +185,10 @@
     <t>DB 5</t>
   </si>
   <si>
-    <t>https://ieeexplore.ieee.org/stamp/stamp.jsp?tp=&amp;arnumber=8840853</t>
-  </si>
-  <si>
     <t>Movements Classification of Multi-Channel sEMG
 Based on CNN and Stacking Ensemble Learning</t>
   </si>
   <si>
-    <t>https://ieeexplore.ieee.org/stamp/stamp.jsp?tp=&amp;arnumber=8900709</t>
-  </si>
-  <si>
     <t xml:space="preserve">On the Use of Deeper CNNs in Hand Gesture
 Recognition Based on sEMG Signals </t>
   </si>
@@ -299,6 +275,487 @@
   </si>
   <si>
     <t>20,54 (4)</t>
+  </si>
+  <si>
+    <t>Performance Evaluation of Convolutional Neural
+Network for Hand Gesture Recognition Using EMG</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/sensors-20-01642%20(2).pdf</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/sensors-20-00969-v2%20(3).pdf</t>
+  </si>
+  <si>
+    <t>Deep Learning in Physiological Signal Data: A Survey</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/symmetry-12-00541-v2.pdf</t>
+  </si>
+  <si>
+    <t>Pattern Recognition of Single-Channel sEMG Signal
+Using PCA and ANN Method to Classify Nine
+Hand Movements</t>
+  </si>
+  <si>
+    <t>Survey paper on hand gesture reconization based on surface EMG sensors</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/1.5112357.pdf</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/applsci-09-04402%20(1).pdf</t>
+  </si>
+  <si>
+    <t>Support Vector Machine-Based EMG Signal Classification Techniques: A Review</t>
+  </si>
+  <si>
+    <t>Biomedical Signal Processing and Control</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/1-s2.0-S1746809419302502-main.pdf</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/sensors-20-00672-v2%20(9).pdf</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/08901936.pdf</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/08630679.pdf</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/08983049.pdf</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/08840853.pdf</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/08900709.pdf</t>
+  </si>
+  <si>
+    <t>The Ninapro Database: a Resource for sEMG Naturally Controlled
+Robotic Hand Prosthetics</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/07320041.pdf</t>
+  </si>
+  <si>
+    <t>Building the NINAPRO Database:
+A Resource for the Biorobotics Community</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/06290287.pdf</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/profile/Henning_Mueller2/publication/261857434_Projet_NinaPro_developper_la_dexterite_d'une_prothese_de_la_main/links/02e7e535ec0121090a000000/Projet-NinaPro-developper-la-dexterite-dune-prothese-de-la-main.pdf</t>
+  </si>
+  <si>
+    <t>Recognition of Hand Movements in a Trans–Radial
+Amputated Subject by sEMG</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/06650486.pdf</t>
+  </si>
+  <si>
+    <t>EMG-based online classification of gestures with recurrent neural networks</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/IJ_39.pdf</t>
+  </si>
+  <si>
+    <t>Comparison of six electromyography acquisition setups on hand movement classification tasks</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/094dea5483184fa9ccba908bc99a8300f85a.pdf</t>
+  </si>
+  <si>
+    <t>Surface-Electromyography-Based Gesture
+Recognition by Multi-View Deep Learning</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/08641445.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convolutional Neural Network Based Human
+Movement Recognition Using Surface
+Electromyography </t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/08713564.pdf</t>
+  </si>
+  <si>
+    <t>Dynamic Gesture Recognition Based on
+LSTM-CNN</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/08623035.pdf</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/08730264.pdf</t>
+  </si>
+  <si>
+    <t>Classifying Hand Movement Intentions Using
+Surface EMG signals and SVM (auf spanisch)</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>ABOUT DATASET</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/s41597-019-0349-2.pdf</t>
+  </si>
+  <si>
+    <t>A large calibrated database of hand movements and grasps kinematics</t>
+  </si>
+  <si>
+    <t>Ex A</t>
+  </si>
+  <si>
+    <t>Ex B</t>
+  </si>
+  <si>
+    <t>Ex C</t>
+  </si>
+  <si>
+    <t>Ex D</t>
+  </si>
+  <si>
+    <t>dynamic</t>
+  </si>
+  <si>
+    <t>static</t>
+  </si>
+  <si>
+    <t>Classifiers</t>
+  </si>
+  <si>
+    <t>SVM(RBF)/MLP/kNN/SVM(linear)/LDA</t>
+  </si>
+  <si>
+    <t>MAV/mDWT/HIST/WL/STFT/VAR/CC</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/699%20(1).pdf</t>
+  </si>
+  <si>
+    <t>IEMG/MAV/MAV1/MAV2/SSI/VAR/WL/ACC</t>
+  </si>
+  <si>
+    <t>Natural Control Capabilities of Robotic Hands by Hand Amputated
+Subjects</t>
+  </si>
+  <si>
+    <t>LDA/LSSVM/RF/kNN</t>
+  </si>
+  <si>
+    <t>HIST/RMS/WL/mDWT</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/stamp/stamp.jsp?tp=&amp;arnumber=6347099</t>
+  </si>
+  <si>
+    <t>60 and 79</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/671%20(1).pdf</t>
+  </si>
+  <si>
+    <t>A Benchmark Database for Myoelectric Movement
+Classification / Characterization of a Benchmark Database
+for Myoelectric Movement Classification</t>
+  </si>
+  <si>
+    <t>12 basic movements of the fingers (flexions and extensions)</t>
+  </si>
+  <si>
+    <t>8 isometric, isotonic hand configurations (”hand postures”); 9 basic movements of the wrist (adduction/abduction,
+flexion/extension and pronation/supination);</t>
+  </si>
+  <si>
+    <t>23 grasping and functional movements — in this case,
+everyday objects are presented to the subject for grasping, in order to mimick a daily-life action.</t>
+  </si>
+  <si>
+    <t>LS-SVM (RBF)</t>
+  </si>
+  <si>
+    <t>Projet NinaPro : développer la dextérité d’une prothèse de la main (auf französisch)</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/sdata201453.pdf</t>
+  </si>
+  <si>
+    <t>Electromyography data for
+non-invasive naturally-controlled
+robotic hand prostheses</t>
+  </si>
+  <si>
+    <t>mDWT</t>
+  </si>
+  <si>
+    <t>about the 3 datasets officiel paper</t>
+  </si>
+  <si>
+    <t>about the 9 datasets officiel paper</t>
+  </si>
+  <si>
+    <t>DB1-DB9</t>
+  </si>
+  <si>
+    <t>DB1-DB3</t>
+  </si>
+  <si>
+    <t>about the 3 datasets, but general setup description is helpful</t>
+  </si>
+  <si>
+    <t>use own data</t>
+  </si>
+  <si>
+    <t>DB1</t>
+  </si>
+  <si>
+    <t>about 1 dataset ML methods comparison</t>
+  </si>
+  <si>
+    <t>experiments devide Ex A and Ex B so number of classes is reduced</t>
+  </si>
+  <si>
+    <t>CNN</t>
+  </si>
+  <si>
+    <t>61,4/ 61,75/58,27</t>
+  </si>
+  <si>
+    <t>LCNN /LDA /SVM</t>
+  </si>
+  <si>
+    <t>CNN features</t>
+  </si>
+  <si>
+    <t>Multi-View CNN</t>
+  </si>
+  <si>
+    <t>uses inter-subject 4-fold cross-validation and solves the distribution difference between train and test sets using multistream AdaBN</t>
+  </si>
+  <si>
+    <t>Ex A,B,C seperate</t>
+  </si>
+  <si>
+    <t>CWT</t>
+  </si>
+  <si>
+    <t>EMGNet (spectrogram CNN)</t>
+  </si>
+  <si>
+    <t>spectrogram</t>
+  </si>
+  <si>
+    <t>CNN-LSTM</t>
+  </si>
+  <si>
+    <t>pick up the classifiers compared to, also talked about the domain adaptation which he did not use</t>
+  </si>
+  <si>
+    <t>ConvNet</t>
+  </si>
+  <si>
+    <t>CWT/Specto/raw/learnable param</t>
+  </si>
+  <si>
+    <t>only ExA + ExB together (41Mov)</t>
+  </si>
+  <si>
+    <t>RMS/TD stats</t>
+  </si>
+  <si>
+    <t>FCNN</t>
+  </si>
+  <si>
+    <t>I/ Intro</t>
+  </si>
+  <si>
+    <t>II/ Related Works</t>
+  </si>
+  <si>
+    <t>III/ Methodology</t>
+  </si>
+  <si>
+    <t>III/ 1. Framework</t>
+  </si>
+  <si>
+    <t>III/ 2. Data und Processing</t>
+  </si>
+  <si>
+    <t>III/ 3. CLASSIC sEMG CLASSIFICATION</t>
+  </si>
+  <si>
+    <t>III/ 4. DEEP LEARNING CLASSIFIERS OVERVIEW (inside proposed)</t>
+  </si>
+  <si>
+    <t>IV/ Results</t>
+  </si>
+  <si>
+    <t>IV/ 1. Dataset</t>
+  </si>
+  <si>
+    <t>IV/ 3. MODEL OPTIMIZATION</t>
+  </si>
+  <si>
+    <t>IV/ 2. Visualization</t>
+  </si>
+  <si>
+    <t>IV/ 4. Comparison of different models</t>
+  </si>
+  <si>
+    <t>V/ Conclusion</t>
+  </si>
+  <si>
+    <t>very good structure/ 4 rep for train, 2 for test</t>
+  </si>
+  <si>
+    <t>Primary/secondary classifier (NN)</t>
+  </si>
+  <si>
+    <t>Time domain, freq domain, time/freq domain</t>
+  </si>
+  <si>
+    <t>repetitions 5 and 9 for train, rest for train</t>
+  </si>
+  <si>
+    <t>images 8x15</t>
+  </si>
+  <si>
+    <t>kNN</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>FFNN/RNN/GRU/LSTM</t>
+  </si>
+  <si>
+    <t>93,75/90,33/91,60/90,83</t>
+  </si>
+  <si>
+    <t>data split 60, 20, 20</t>
+  </si>
+  <si>
+    <t>own dataset</t>
+  </si>
+  <si>
+    <t>survey</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>CNN/RNN</t>
+  </si>
+  <si>
+    <t>no idea</t>
+  </si>
+  <si>
+    <t>16 features</t>
+  </si>
+  <si>
+    <t>FNN</t>
+  </si>
+  <si>
+    <t>description of features</t>
+  </si>
+  <si>
+    <t>MAV/RMD/AutoReg/Var/std/WL/ZC/Wavelet</t>
+  </si>
+  <si>
+    <t>SVM methods, good description of other works</t>
+  </si>
+  <si>
+    <t>data of Khushaba et al</t>
+  </si>
+  <si>
+    <t>6 features</t>
+  </si>
+  <si>
+    <t>8 classes</t>
+  </si>
+  <si>
+    <t>NN/SVM/RF/DT/kNN</t>
+  </si>
+  <si>
+    <t>2019_surface_huang</t>
+  </si>
+  <si>
+    <t>2020_hand_chen</t>
+  </si>
+  <si>
+    <t>2019_deep_chaiyaroj</t>
+  </si>
+  <si>
+    <t>2019_emg_simao</t>
+  </si>
+  <si>
+    <t>2018_convolutional_ruan</t>
+  </si>
+  <si>
+    <t>Wavelet packet transform (TD/FD)</t>
+  </si>
+  <si>
+    <t>2014_natural_atzori</t>
+  </si>
+  <si>
+    <t>2018_dynamic_wu</t>
+  </si>
+  <si>
+    <t>On the Challenge of Classifying 52 Hand Movements from Surface
+Electromyography</t>
+  </si>
+  <si>
+    <t>db5</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/ussema/Downloads/06347099.pdf</t>
+  </si>
+  <si>
+    <t>ts</t>
+  </si>
+  <si>
+    <t>mdwt</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>scat1d</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>specs</t>
+  </si>
+  <si>
+    <t>inter-subject / intra-subject</t>
+  </si>
+  <si>
+    <t>69.18 (9)</t>
+  </si>
+  <si>
+    <t>85.04 (50)</t>
+  </si>
+  <si>
+    <t>2019_surface_wei</t>
+  </si>
+  <si>
+    <t>2017_comparison_stefano</t>
+  </si>
+  <si>
+    <t>2012_building_atzori</t>
+  </si>
+  <si>
+    <t>2019_movements_shen</t>
   </si>
 </sst>
 </file>
@@ -339,15 +796,39 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -355,12 +836,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -368,10 +864,34 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -747,24 +1267,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:S80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="8" max="8" width="90.15234375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.84375" customWidth="1"/>
+    <col min="11" max="11" width="11.3046875" customWidth="1"/>
+    <col min="12" max="12" width="16.61328125" customWidth="1"/>
+    <col min="13" max="13" width="19.07421875" customWidth="1"/>
+    <col min="14" max="14" width="8.61328125" customWidth="1"/>
+    <col min="15" max="15" width="83.61328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
@@ -810,6 +1337,9 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="B4">
+        <v>56.34</v>
+      </c>
       <c r="C4">
         <v>38.58</v>
       </c>
@@ -880,7 +1410,7 @@
         <v>26</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
@@ -899,17 +1429,17 @@
       <c r="E8" t="s">
         <v>30</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B10" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
@@ -1027,11 +1557,11 @@
       <c r="E16" t="s">
         <v>26</v>
       </c>
-      <c r="F16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F16" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1051,15 +1581,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B19" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B19" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1079,7 +1609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1090,16 +1620,16 @@
         <v>14.8</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+        <v>66</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1110,16 +1640,16 @@
         <v>14.95</v>
       </c>
       <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E22" t="s">
-        <v>75</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1130,16 +1660,16 @@
         <v>15.03</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E23" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1149,14 +1679,17 @@
       <c r="C24" s="2">
         <v>13.4</v>
       </c>
+      <c r="D24" s="18">
+        <v>11.93</v>
+      </c>
       <c r="E24" t="s">
-        <v>77</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+        <v>69</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1167,13 +1700,13 @@
         <v>11.07</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1184,21 +1717,21 @@
         <v>14.95</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B28" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B28" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -1218,7 +1751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1229,16 +1762,16 @@
         <v>0.15670000000000001</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E30" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -1257,8 +1790,11 @@
       <c r="F31" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="H31" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1269,16 +1805,41 @@
         <v>0.20530000000000001</v>
       </c>
       <c r="D32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E32" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="H32" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="I32">
+        <v>2014</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N32" s="3"/>
+      <c r="O32" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="P32" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -1289,13 +1850,35 @@
         <v>0.2319</v>
       </c>
       <c r="E33" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.4">
+        <v>60</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="I33">
+        <v>2019</v>
+      </c>
+      <c r="J33" s="3"/>
+      <c r="K33" s="17">
+        <v>55</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O33" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1306,13 +1889,43 @@
         <v>0.1081</v>
       </c>
       <c r="E34" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.4">
+        <v>62</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="I34">
+        <v>2018</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O34" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="P34" t="s">
+        <v>215</v>
+      </c>
+      <c r="S34" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -1331,104 +1944,745 @@
       <c r="F35" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="H39" s="3" t="s">
+      <c r="H35" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="I35">
+        <v>2018</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3">
+        <v>90.77</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="N35" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O35" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="P35" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="H36" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I36">
+        <v>2019</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="K36" s="16">
+        <v>90</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="N36" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="O36" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="P36" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>219</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I37">
+        <v>2020</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="K37" s="16">
+        <v>69.62</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O37" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="P37" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>220</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I38">
+        <v>2019</v>
+      </c>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3">
+        <v>79.328999999999994</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="M38" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="N38" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O38" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="P38" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>221</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>45</v>
+      </c>
       <c r="I39">
-        <v>2020</v>
-      </c>
-      <c r="J39">
-        <v>69.62</v>
-      </c>
-      <c r="K39" t="s">
+        <v>2019</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="K39" s="17">
+        <v>68.98</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="N39" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O39" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>222</v>
+      </c>
+      <c r="H40" s="13" t="s">
         <v>46</v>
-      </c>
-      <c r="L39" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="H40" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="I40">
         <v>2019</v>
       </c>
-      <c r="J40">
-        <v>79.328999999999994</v>
-      </c>
-      <c r="K40" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="H41" s="3" t="s">
-        <v>49</v>
+      <c r="J40" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="K40" s="16">
+        <v>91</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="N40" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O40" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="P40" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>223</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="I41">
         <v>2019</v>
       </c>
-      <c r="J41">
-        <v>68.98</v>
-      </c>
-      <c r="K41" t="s">
-        <v>46</v>
-      </c>
-      <c r="L41" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="H42" s="3" t="s">
-        <v>52</v>
+      <c r="J41" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="K41" s="16">
+        <v>72.09</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O41" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="P41" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>224</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="I42">
         <v>2019</v>
       </c>
-      <c r="J42">
-        <v>0.91</v>
-      </c>
-      <c r="K42" t="s">
-        <v>50</v>
-      </c>
-      <c r="L42" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="H43" s="3" t="s">
-        <v>55</v>
+      <c r="J42" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K42" s="17">
+        <v>55.31</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O42" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="H43" s="11" t="s">
+        <v>101</v>
       </c>
       <c r="I43">
-        <v>2019</v>
-      </c>
-      <c r="J43">
-        <v>0.72</v>
-      </c>
-      <c r="K43" t="s">
-        <v>53</v>
-      </c>
-      <c r="L43" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="H44" s="3" t="s">
-        <v>57</v>
+        <v>2013</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K43" s="3">
+        <v>61.5</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="O43" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="H44" s="13" t="s">
+        <v>103</v>
       </c>
       <c r="I44">
         <v>2019</v>
       </c>
-      <c r="J44">
-        <v>0.55310000000000004</v>
-      </c>
-      <c r="K44" t="s">
-        <v>46</v>
-      </c>
-      <c r="L44" s="4" t="s">
-        <v>56</v>
+      <c r="J44" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="M44" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="N44" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O44" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="P44" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="H45" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I45">
+        <v>2020</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N45" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="O45" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="H46" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I46">
+        <v>2020</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="K46" s="3">
+        <v>87.3</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N46" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="O46" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="H47" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="I47">
+        <v>2020</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="K47" s="3">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="L47" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="M47" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="N47" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="O47" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="H48" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="I48">
+        <v>2019</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="M48" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="O48" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="H49" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I49">
+        <v>2019</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="O49" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="H50" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="I50">
+        <v>2019</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="K50" s="3">
+        <v>91.78</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="M50" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="N50" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="O50" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="H51" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="I51">
+        <v>2012</v>
+      </c>
+      <c r="J51" s="3">
+        <v>53</v>
+      </c>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="O51" s="15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="H52" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+    </row>
+    <row r="53" spans="1:16" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="H53" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="H54" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="I54">
+        <v>2012</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="K54" s="16">
+        <v>79.7</v>
+      </c>
+      <c r="L54" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O54" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="P54" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="H55" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="O55" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="H56" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="I56">
+        <v>2017</v>
+      </c>
+      <c r="J56" s="3"/>
+      <c r="K56" s="17">
+        <v>69.040000000000006</v>
+      </c>
+      <c r="L56" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="M56" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="N56" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O56" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="P56" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="H57" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="I57">
+        <v>2020</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="O57" s="15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="H58" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="I58">
+        <v>2014</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="O58" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="H59" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="I59">
+        <v>2015</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="K59" s="3">
+        <v>76</v>
+      </c>
+      <c r="L59" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="M59" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="N59" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="O59" s="15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A64" t="s">
+        <v>119</v>
+      </c>
+      <c r="C64" s="7">
+        <v>12</v>
+      </c>
+      <c r="D64" t="s">
+        <v>124</v>
+      </c>
+      <c r="E64" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A65" t="s">
+        <v>120</v>
+      </c>
+      <c r="C65" s="7">
+        <v>17</v>
+      </c>
+      <c r="D65" t="s">
+        <v>124</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A66" t="s">
+        <v>121</v>
+      </c>
+      <c r="C66" s="7">
+        <v>23</v>
+      </c>
+      <c r="D66" t="s">
+        <v>124</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A67" t="s">
+        <v>122</v>
+      </c>
+      <c r="C67">
+        <v>9</v>
+      </c>
+      <c r="D67" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H68" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H69" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H70" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H71" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H72" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H73" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H74" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H75" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H76" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H77" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H79" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H80" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -1439,19 +2693,42 @@
     <mergeCell ref="B28:E28"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="L39" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="L41" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="L42" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="L43" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="L44" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="O37" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="O39" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="O40" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="O41" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="O42" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="O45" r:id="rId6" xr:uid="{06F6A9C4-B584-4967-8BCD-AA0E4B4BA622}"/>
+    <hyperlink ref="O46" r:id="rId7" xr:uid="{D22D8B45-242E-4711-A3F0-4C71525D2BBA}"/>
+    <hyperlink ref="O48" r:id="rId8" xr:uid="{A7F0CEEB-A54E-4289-BA78-4C2B724D4B34}"/>
+    <hyperlink ref="O49" r:id="rId9" xr:uid="{F60246AB-4B09-4216-9CA3-C9FB92B04469}"/>
+    <hyperlink ref="O50" r:id="rId10" xr:uid="{7141C66E-3FC6-4553-A1CE-9798F37AF531}"/>
+    <hyperlink ref="O38" r:id="rId11" xr:uid="{4653B410-49E0-44AD-8F0F-1B79BA03F5A6}"/>
+    <hyperlink ref="O53" r:id="rId12" xr:uid="{E28BF022-FB08-4629-9C70-26CD55D5C89B}"/>
+    <hyperlink ref="O54" r:id="rId13" xr:uid="{1352AB82-A80B-4CD2-9ECC-00A9162D9DF8}"/>
+    <hyperlink ref="O55" r:id="rId14" xr:uid="{37B78B41-E3FE-43F9-BC6A-AB4FCA54384F}"/>
+    <hyperlink ref="O43" r:id="rId15" xr:uid="{0330D105-3AD7-48AD-A158-54BE28BC05B6}"/>
+    <hyperlink ref="O44" r:id="rId16" xr:uid="{8EB6F620-12F6-4C09-92A2-5D735BD69169}"/>
+    <hyperlink ref="O56" r:id="rId17" display="C:\Users\ussema\Downloads\094dea5483184fa9ccba908bc99a8300f85a.pdf" xr:uid="{ADC4F4F2-67A4-43B5-A773-69EF2B4EAEDF}"/>
+    <hyperlink ref="O36" r:id="rId18" display="C:\Users\ussema\Downloads\08641445.pdf" xr:uid="{0035D855-AD78-45A0-A486-4BC93078AA33}"/>
+    <hyperlink ref="O35" r:id="rId19" xr:uid="{C964EB67-4B86-466F-A5E4-11396EA00BE1}"/>
+    <hyperlink ref="O34" r:id="rId20" xr:uid="{EBC2FFE4-BAAF-4C73-8A21-9343E889DC11}"/>
+    <hyperlink ref="O33" r:id="rId21" xr:uid="{4ABD7DC0-7E80-4931-94AA-DE8D1D6A4B06}"/>
+    <hyperlink ref="O57" r:id="rId22" xr:uid="{5BAC557C-113C-4772-8855-299D98C8152F}"/>
+    <hyperlink ref="O59" r:id="rId23" xr:uid="{55F1905F-1F46-429A-A316-BA238D38104C}"/>
+    <hyperlink ref="S34" r:id="rId24" xr:uid="{B0CEAC8A-7C80-4ED2-8DCB-CCF08FF61FCB}"/>
+    <hyperlink ref="O32" r:id="rId25" xr:uid="{E9625A4E-F387-4248-B931-371519693D7C}"/>
+    <hyperlink ref="O58" r:id="rId26" display="C:\Users\ussema\Downloads\sdata201453.pdf" xr:uid="{458C97A2-7CEA-4AD1-9258-1BD0204F23BF}"/>
+    <hyperlink ref="O47" r:id="rId27" xr:uid="{B8DCD6CB-BDCC-4E0F-8D89-1B3B148A1C02}"/>
+    <hyperlink ref="O51" r:id="rId28" xr:uid="{3943A3BB-B311-489F-B9FE-1FC82C59576D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
   <tableParts count="4">
-    <tablePart r:id="rId7"/>
-    <tablePart r:id="rId8"/>
-    <tablePart r:id="rId9"/>
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId30"/>
+    <tablePart r:id="rId31"/>
+    <tablePart r:id="rId32"/>
+    <tablePart r:id="rId33"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>